<commit_message>
test optimize plugin and various...
</commit_message>
<xml_diff>
--- a/projects/fr/docs/assets/tables/GDMBR.xlsx
+++ b/projects/fr/docs/assets/tables/GDMBR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gravel/Private/f3/projects/fr/docs/assets/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E5AA18-FC4D-084C-8589-817EC57594B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323D67A7-04CF-7440-93E8-BA4EC883AB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="760" windowWidth="33860" windowHeight="23260" xr2:uid="{3D076BE0-CA79-3448-855F-AD0FA0DCE9D7}"/>
   </bookViews>
@@ -1436,7 +1436,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1455,6 +1455,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1469,7 +1481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1499,6 +1511,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1837,7 +1854,7 @@
   <dimension ref="A1:AI56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2013,7 +2030,7 @@
       <c r="B3" s="5">
         <v>45541.271261574075</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="25" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="5" t="str">
@@ -2026,7 +2043,7 @@
       <c r="F3" t="s">
         <v>196</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="21" t="s">
         <v>239</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -2136,7 +2153,7 @@
       <c r="F4" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="21" t="s">
         <v>137</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -2247,7 +2264,7 @@
       <c r="F5" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="21" t="s">
         <v>240</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -2358,7 +2375,7 @@
       <c r="F6" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="21" t="s">
         <v>141</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -2469,7 +2486,7 @@
       <c r="F7" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="21" t="s">
         <v>241</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -2580,7 +2597,7 @@
       <c r="F8" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="21" t="s">
         <v>143</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -2691,7 +2708,7 @@
       <c r="F9" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="21" t="s">
         <v>242</v>
       </c>
       <c r="H9" s="5" t="s">
@@ -2802,7 +2819,7 @@
       <c r="F10" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="21" t="s">
         <v>243</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -2913,7 +2930,7 @@
       <c r="F11" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="21" t="s">
         <v>244</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -3024,7 +3041,7 @@
       <c r="F12" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="21" t="s">
         <v>245</v>
       </c>
       <c r="H12" s="5" t="s">
@@ -3135,7 +3152,7 @@
       <c r="F13" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="21" t="s">
         <v>246</v>
       </c>
       <c r="H13" s="5" t="s">
@@ -3246,7 +3263,7 @@
       <c r="F14" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="21" t="s">
         <v>247</v>
       </c>
       <c r="H14" s="5" t="s">
@@ -3357,7 +3374,7 @@
       <c r="F15" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="21" t="s">
         <v>248</v>
       </c>
       <c r="H15" s="5"/>
@@ -3452,7 +3469,7 @@
       <c r="B16" s="5">
         <v>45528.701655092591</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="24" t="s">
         <v>116</v>
       </c>
       <c r="D16" s="5" t="str">
@@ -3463,7 +3480,7 @@
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="21" t="s">
         <v>278</v>
       </c>
       <c r="H16" s="5" t="s">
@@ -3574,7 +3591,7 @@
       <c r="F17" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="21" t="s">
         <v>249</v>
       </c>
       <c r="H17" s="5" t="s">
@@ -3685,7 +3702,7 @@
       <c r="F18" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="21" t="s">
         <v>250</v>
       </c>
       <c r="H18" s="5" t="s">
@@ -3796,7 +3813,7 @@
       <c r="F19" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="21" t="s">
         <v>251</v>
       </c>
       <c r="H19" s="5" t="s">
@@ -3907,7 +3924,7 @@
       <c r="F20" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="21" t="s">
         <v>252</v>
       </c>
       <c r="H20" s="5" t="s">
@@ -4018,7 +4035,7 @@
       <c r="F21" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="21" t="s">
         <v>253</v>
       </c>
       <c r="H21" s="5" t="s">
@@ -4115,7 +4132,7 @@
       <c r="B22" s="5">
         <v>45522.654398148145</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="23" t="s">
         <v>116</v>
       </c>
       <c r="D22" s="5" t="str">
@@ -4129,7 +4146,7 @@
       <c r="F22" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="21" t="s">
         <v>254</v>
       </c>
       <c r="H22" s="5" t="s">
@@ -4240,7 +4257,7 @@
       <c r="F23" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="21" t="s">
         <v>255</v>
       </c>
       <c r="H23" s="5" t="s">
@@ -4351,7 +4368,7 @@
       <c r="F24" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="21" t="s">
         <v>256</v>
       </c>
       <c r="H24" s="5" t="s">
@@ -4462,7 +4479,7 @@
       <c r="F25" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="21" t="s">
         <v>257</v>
       </c>
       <c r="H25" s="5" t="s">
@@ -4573,7 +4590,7 @@
       <c r="F26" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="21" t="s">
         <v>258</v>
       </c>
       <c r="H26" s="5" t="s">
@@ -4684,7 +4701,7 @@
       <c r="F27" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="21" t="s">
         <v>259</v>
       </c>
       <c r="H27" s="5" t="s">
@@ -4795,7 +4812,7 @@
       <c r="F28" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="21" t="s">
         <v>260</v>
       </c>
       <c r="H28" s="5" t="s">
@@ -4906,7 +4923,7 @@
       <c r="F29" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="21" t="s">
         <v>261</v>
       </c>
       <c r="H29" s="5" t="s">
@@ -5017,7 +5034,7 @@
       <c r="F30" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="21" t="s">
         <v>262</v>
       </c>
       <c r="H30" s="5" t="s">
@@ -5128,7 +5145,7 @@
       <c r="F31" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="21" t="s">
         <v>263</v>
       </c>
       <c r="H31" s="5" t="s">
@@ -5239,7 +5256,7 @@
       <c r="F32" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="21" t="s">
         <v>264</v>
       </c>
       <c r="H32" s="5" t="s">
@@ -5350,7 +5367,7 @@
       <c r="F33" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="21" t="s">
         <v>265</v>
       </c>
       <c r="H33" s="5" t="s">
@@ -5461,7 +5478,7 @@
       <c r="F34" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="21" t="s">
         <v>266</v>
       </c>
       <c r="H34" s="5" t="s">
@@ -5557,7 +5574,7 @@
       <c r="B35" s="20">
         <v>45509</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="22" t="s">
         <v>109</v>
       </c>
       <c r="D35" s="5" t="str">
@@ -5570,7 +5587,7 @@
       <c r="F35" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="21" t="s">
         <v>267</v>
       </c>
       <c r="H35" s="5" t="s">
@@ -5631,7 +5648,7 @@
       <c r="F36" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="21" t="s">
         <v>268</v>
       </c>
       <c r="H36" s="5" t="s">
@@ -5741,7 +5758,7 @@
       <c r="F37" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="21" t="s">
         <v>269</v>
       </c>
       <c r="H37" s="5" t="s">
@@ -5851,7 +5868,7 @@
       <c r="F38" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="21" t="s">
         <v>270</v>
       </c>
       <c r="H38" s="5" t="s">
@@ -5961,7 +5978,7 @@
       <c r="F39" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="21" t="s">
         <v>271</v>
       </c>
       <c r="H39" s="5" t="s">
@@ -6071,7 +6088,7 @@
       <c r="F40" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="21" t="s">
         <v>272</v>
       </c>
       <c r="H40" s="5" t="s">
@@ -6181,7 +6198,7 @@
       <c r="F41" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="21" t="s">
         <v>273</v>
       </c>
       <c r="H41" s="5" t="s">
@@ -6291,7 +6308,7 @@
       <c r="F42" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="21" t="s">
         <v>274</v>
       </c>
       <c r="H42" s="5" t="s">
@@ -6388,7 +6405,7 @@
       <c r="B43" s="5">
         <v>45501.56591435185</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="23" t="s">
         <v>116</v>
       </c>
       <c r="D43" s="5" t="str">
@@ -6401,7 +6418,7 @@
       <c r="F43" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="21" t="s">
         <v>275</v>
       </c>
       <c r="H43" s="5" t="s">

</xml_diff>